<commit_message>
Added Board Creation of .NET/JAVA boards and cards
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Revature Training\Myrepo\Thomas-Vo\Trello Backlog NextGen Automation\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Revature-Capstone-1362\construct-trello-boards\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{981BA3B7-29B1-487D-8BE9-58F0755857F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{088C7E40-B4C1-4411-957A-84A2B914D201}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6930" yWindow="4350" windowWidth="22095" windowHeight="15660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2370" yWindow="3870" windowWidth="23550" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -123,7 +123,7 @@
     <t>Trello Mock Data</t>
   </si>
   <si>
-    <t>Mock Data</t>
+    <t>TrelloTest</t>
   </si>
 </sst>
 </file>
@@ -502,7 +502,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
Modified config file to update Queue Name
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Revature-Capstone-1362\construct-trello-boards\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{088C7E40-B4C1-4411-957A-84A2B914D201}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CE6DD32-87C6-4790-A377-344F328C24A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2370" yWindow="3870" windowWidth="23550" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3450" yWindow="6180" windowWidth="28185" windowHeight="11265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -123,14 +123,14 @@
     <t>Trello Mock Data</t>
   </si>
   <si>
-    <t>TrelloTest</t>
+    <t>Revature Associates</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -154,6 +154,13 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF464E55"/>
+      <name val="Noto Sans"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -175,7 +182,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -185,6 +192,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -551,7 +559,7 @@
       <c r="A2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="5" t="s">
         <v>32</v>
       </c>
       <c r="C2" s="2" t="s">

</xml_diff>

<commit_message>
Move some settings to config file
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Revature-Capstone-1362\construct-trello-boards\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Revature\Revature-Capstone-1362\construct-trello-boards\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CE6DD32-87C6-4790-A377-344F328C24A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76D497DC-4802-47C9-AC8E-CC35EBFCC8C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3450" yWindow="6180" windowWidth="28185" windowHeight="11265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
   <si>
     <t>Name</t>
   </si>
@@ -124,6 +124,18 @@
   </si>
   <si>
     <t>Revature Associates</t>
+  </si>
+  <si>
+    <t>BoardListPath</t>
+  </si>
+  <si>
+    <t>InputDataPath</t>
+  </si>
+  <si>
+    <t>D:\Revature\Revature-Capstone-1362\construct-trello-boards\Trello Backlog Dispatcher\MockData.xlsx</t>
+  </si>
+  <si>
+    <t>D:\Revature\Revature-Capstone-1362\construct-trello-boards\Trello Backlog Dispatcher\BoardList.xlsx</t>
   </si>
 </sst>
 </file>
@@ -507,10 +519,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z997"/>
+  <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -566,19 +578,33 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="4" spans="1:26" ht="30">
+    <row r="3" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="30">
+      <c r="A5" t="s">
         <v>20</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C5" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1571,6 +1597,7 @@
     <row r="995" ht="14.25" customHeight="1"/>
     <row r="996" ht="14.25" customHeight="1"/>
     <row r="997" ht="14.25" customHeight="1"/>
+    <row r="998" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>